<commit_message>
Se suben últimos cambios antes del cambio de compu
</commit_message>
<xml_diff>
--- a/Revisión-Precios-API/Dealers.xlsx
+++ b/Revisión-Precios-API/Dealers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvelasc2\source\repos\Revisión-Precios-API\Revisión-Precios-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14891710-0B00-45D2-ABF6-E0CE2F6326CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C21163C-2AC9-4158-B2EC-3F1CD49CBA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="27151" windowHeight="16927" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="123">
   <si>
     <t>VERIFICAR</t>
   </si>
@@ -301,106 +301,94 @@
     <t>1,061,000</t>
   </si>
   <si>
+    <t>330,900</t>
+  </si>
+  <si>
+    <t>370,900</t>
+  </si>
+  <si>
+    <t>398,900</t>
+  </si>
+  <si>
+    <t>403,900</t>
+  </si>
+  <si>
+    <t>442,900</t>
+  </si>
+  <si>
+    <t>482,900</t>
+  </si>
+  <si>
+    <t>458,900</t>
+  </si>
+  <si>
+    <t>498,900</t>
+  </si>
+  <si>
+    <t>568,900</t>
+  </si>
+  <si>
+    <t>391,900</t>
+  </si>
+  <si>
+    <t>421,900</t>
+  </si>
+  <si>
+    <t>441,900</t>
+  </si>
+  <si>
+    <t>471,900</t>
+  </si>
+  <si>
+    <t>517,900</t>
+  </si>
+  <si>
+    <t>557,900</t>
+  </si>
+  <si>
+    <t>551,900</t>
+  </si>
+  <si>
+    <t>611,900</t>
+  </si>
+  <si>
+    <t>681,900</t>
+  </si>
+  <si>
+    <t>818,900</t>
+  </si>
+  <si>
+    <t>961,000</t>
+  </si>
+  <si>
+    <t>529,900</t>
+  </si>
+  <si>
+    <t>629,900</t>
+  </si>
+  <si>
+    <t>mazda-cx-70-racks-flydown-inclinado-v1</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>PICKUPS</t>
+  </si>
+  <si>
+    <t>MAZDA BT-50</t>
+  </si>
+  <si>
+    <t>mazda-bt-50-roja-flydown-inclinado-v2</t>
+  </si>
+  <si>
+    <t>3.0L</t>
+  </si>
+  <si>
     <t>300,900</t>
   </si>
   <si>
-    <t>330,900</t>
-  </si>
-  <si>
-    <t>370,900</t>
-  </si>
-  <si>
-    <t>398,900</t>
-  </si>
-  <si>
-    <t>403,900</t>
-  </si>
-  <si>
-    <t>442,900</t>
-  </si>
-  <si>
-    <t>482,900</t>
-  </si>
-  <si>
-    <t>458,900</t>
-  </si>
-  <si>
-    <t>498,900</t>
-  </si>
-  <si>
-    <t>568,900</t>
-  </si>
-  <si>
-    <t>391,900</t>
-  </si>
-  <si>
-    <t>421,900</t>
-  </si>
-  <si>
-    <t>441,900</t>
-  </si>
-  <si>
-    <t>471,900</t>
-  </si>
-  <si>
-    <t>517,900</t>
-  </si>
-  <si>
-    <t>557,900</t>
-  </si>
-  <si>
-    <t>551,900</t>
-  </si>
-  <si>
-    <t>611,900</t>
-  </si>
-  <si>
-    <t>681,900</t>
-  </si>
-  <si>
-    <t>818,900</t>
-  </si>
-  <si>
-    <t>961,000</t>
-  </si>
-  <si>
-    <t>529,900</t>
-  </si>
-  <si>
-    <t>629,900</t>
-  </si>
-  <si>
-    <t>mazda-cx-70-racks-flydown-inclinado-v1</t>
-  </si>
-  <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>PICKUPS</t>
-  </si>
-  <si>
-    <t>MAZDA BT-50</t>
-  </si>
-  <si>
-    <t>mazda-bt-50-roja-flydown-inclinado-v2</t>
-  </si>
-  <si>
-    <t>3.0L</t>
-  </si>
-  <si>
-    <t>829,900</t>
-  </si>
-  <si>
-    <t>mazda-mx-5-35-aniversario-flydown-perspectiva-v1</t>
-  </si>
-  <si>
-    <t>MAZDA MX-5 35° ANIVERSARIO</t>
-  </si>
-  <si>
-    <t>639,900</t>
-  </si>
-  <si>
-    <t>35° ANIVERSARIO</t>
+    <t>799,900</t>
   </si>
 </sst>
 </file>
@@ -723,36 +711,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ15"/>
+  <dimension ref="A1:AJ14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.75" customWidth="1"/>
-    <col min="2" max="2" width="30.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.75" customWidth="1"/>
-    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.75" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="13.25" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" customWidth="1"/>
     <col min="8" max="8" width="9" style="1"/>
     <col min="9" max="9" width="4" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.75" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.25" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.25" customWidth="1"/>
+    <col min="10" max="10" width="8.77734375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.21875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.21875" customWidth="1"/>
     <col min="13" max="13" width="9" style="1"/>
-    <col min="14" max="15" width="8.75" style="1"/>
-    <col min="16" max="16" width="9.25" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.75" customWidth="1"/>
+    <col min="14" max="15" width="8.77734375" style="1"/>
+    <col min="16" max="16" width="9.21875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.77734375" customWidth="1"/>
     <col min="18" max="18" width="9" style="1"/>
-    <col min="19" max="21" width="8.75" style="1"/>
-    <col min="22" max="22" width="13.875" customWidth="1"/>
-    <col min="25" max="25" width="8.75" customWidth="1"/>
-    <col min="27" max="27" width="10.125" customWidth="1"/>
-    <col min="32" max="32" width="13.875" customWidth="1"/>
+    <col min="19" max="21" width="8.77734375" style="1"/>
+    <col min="22" max="22" width="13.88671875" customWidth="1"/>
+    <col min="25" max="25" width="8.77734375" customWidth="1"/>
+    <col min="27" max="27" width="10.109375" customWidth="1"/>
+    <col min="32" max="32" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -867,7 +855,7 @@
     </row>
     <row r="2" spans="1:36">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>86</v>
@@ -888,7 +876,7 @@
         <v>37</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>38</v>
@@ -903,7 +891,7 @@
         <v>41</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>38</v>
@@ -918,7 +906,7 @@
         <v>49</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>38</v>
@@ -933,7 +921,7 @@
         <v>50</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>73</v>
@@ -947,7 +935,7 @@
     </row>
     <row r="3" spans="1:36">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>87</v>
@@ -968,7 +956,7 @@
         <v>41</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>38</v>
@@ -983,7 +971,7 @@
         <v>49</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>38</v>
@@ -998,7 +986,7 @@
         <v>50</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>73</v>
@@ -1015,7 +1003,7 @@
     </row>
     <row r="4" spans="1:36">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>89</v>
@@ -1036,7 +1024,7 @@
         <v>37</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>45</v>
@@ -1051,7 +1039,7 @@
         <v>41</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>45</v>
@@ -1066,7 +1054,7 @@
         <v>49</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>45</v>
@@ -1101,7 +1089,7 @@
     </row>
     <row r="5" spans="1:36">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>80</v>
@@ -1122,7 +1110,7 @@
         <v>41</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>45</v>
@@ -1137,7 +1125,7 @@
         <v>49</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>45</v>
@@ -1152,7 +1140,7 @@
         <v>50</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>51</v>
@@ -1171,7 +1159,7 @@
     </row>
     <row r="6" spans="1:36">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>88</v>
@@ -1192,7 +1180,7 @@
         <v>37</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>47</v>
@@ -1207,7 +1195,7 @@
         <v>41</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>47</v>
@@ -1225,7 +1213,7 @@
     </row>
     <row r="7" spans="1:36">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>84</v>
@@ -1246,7 +1234,7 @@
         <v>37</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>45</v>
@@ -1261,7 +1249,7 @@
         <v>41</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>45</v>
@@ -1276,7 +1264,7 @@
         <v>49</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>45</v>
@@ -1291,7 +1279,7 @@
         <v>50</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X7" s="1" t="s">
         <v>51</v>
@@ -1305,7 +1293,7 @@
     </row>
     <row r="8" spans="1:36">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>70</v>
@@ -1326,7 +1314,7 @@
         <v>41</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>58</v>
@@ -1341,7 +1329,7 @@
         <v>49</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>58</v>
@@ -1356,7 +1344,7 @@
         <v>50</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>51</v>
@@ -1374,7 +1362,7 @@
     </row>
     <row r="9" spans="1:36">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>85</v>
@@ -1395,7 +1383,7 @@
         <v>50</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>59</v>
@@ -1409,10 +1397,10 @@
     </row>
     <row r="10" spans="1:36">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>65</v>
@@ -1430,7 +1418,7 @@
         <v>42</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>81</v>
@@ -1444,7 +1432,7 @@
     </row>
     <row r="11" spans="1:36">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>90</v>
@@ -1479,16 +1467,16 @@
     </row>
     <row r="12" spans="1:36">
       <c r="A12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E12" t="s">
         <v>54</v>
@@ -1509,12 +1497,12 @@
         <v>82</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:36">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>71</v>
@@ -1535,7 +1523,7 @@
         <v>41</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>61</v>
@@ -1570,7 +1558,7 @@
         <v>49</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>61</v>
@@ -1579,41 +1567,6 @@
         <v>62</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:36">
-      <c r="A15" t="s">
-        <v>117</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" t="s">
-        <v>124</v>
-      </c>
-      <c r="E15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15">
-        <v>2025</v>
-      </c>
-      <c r="G15" t="s">
-        <v>126</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K15" s="1" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se sube versión actualizada del código, agregando linea para abrir la versión del navegador que se tenga: 06022026
</commit_message>
<xml_diff>
--- a/Revisión-Precios-API/Dealers.xlsx
+++ b/Revisión-Precios-API/Dealers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvelasc2\source\repos\Revisión-Precios-API\Revisión-Precios-API\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manuelvelasco\source\repos\Mvelasco-git\PreciosAPI\Revisión-Precios-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C21163C-2AC9-4158-B2EC-3F1CD49CBA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7558D67F-FF37-4CC4-B6AA-16184233A2AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="27151" windowHeight="16927" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="126">
   <si>
     <t>VERIFICAR</t>
   </si>
@@ -232,163 +232,172 @@
     <t>CATEGORIA</t>
   </si>
   <si>
-    <t>cx-5-flydown-perfil-v1</t>
-  </si>
-  <si>
-    <t>mx-5-carro-rojo-deportivo</t>
-  </si>
-  <si>
-    <t>carro-mazda-mx-5-gris-v1</t>
-  </si>
-  <si>
     <t>141</t>
   </si>
   <si>
     <t>137</t>
   </si>
   <si>
+    <t>340</t>
+  </si>
+  <si>
+    <t>369</t>
+  </si>
+  <si>
+    <t>3.3L</t>
+  </si>
+  <si>
+    <t>MAZDA CX-70</t>
+  </si>
+  <si>
+    <t>mazda3-hatchback-flydown-inclinado-v1</t>
+  </si>
+  <si>
+    <t>280</t>
+  </si>
+  <si>
+    <t>332</t>
+  </si>
+  <si>
+    <t>552,900</t>
+  </si>
+  <si>
+    <t>mazda3-sedan-flydown-perfil-v2</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>398,900</t>
+  </si>
+  <si>
+    <t>403,900</t>
+  </si>
+  <si>
+    <t>442,900</t>
+  </si>
+  <si>
+    <t>482,900</t>
+  </si>
+  <si>
+    <t>458,900</t>
+  </si>
+  <si>
+    <t>498,900</t>
+  </si>
+  <si>
+    <t>568,900</t>
+  </si>
+  <si>
+    <t>551,900</t>
+  </si>
+  <si>
+    <t>611,900</t>
+  </si>
+  <si>
+    <t>681,900</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>PICKUPS</t>
+  </si>
+  <si>
+    <t>MAZDA BT-50</t>
+  </si>
+  <si>
+    <t>mazda-bt-50-roja-flydown-inclinado-v2</t>
+  </si>
+  <si>
+    <t>3.0L</t>
+  </si>
+  <si>
+    <t>mazda2-sedan-rojo-auto-perfil-v1</t>
+  </si>
+  <si>
+    <t>mazda2-hatchback-flydown-perfil-v1</t>
+  </si>
+  <si>
+    <t>301,900</t>
+  </si>
+  <si>
+    <t>331,900</t>
+  </si>
+  <si>
+    <t>371,900</t>
+  </si>
+  <si>
+    <t>502,900</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>432,900</t>
+  </si>
+  <si>
+    <t>451,900</t>
+  </si>
+  <si>
+    <t>481,900</t>
+  </si>
+  <si>
+    <t>525,900</t>
+  </si>
+  <si>
+    <t>577,900</t>
+  </si>
+  <si>
+    <t>837,900</t>
+  </si>
+  <si>
+    <t>996,900</t>
+  </si>
+  <si>
+    <t>1,011,900</t>
+  </si>
+  <si>
+    <t>829,900</t>
+  </si>
+  <si>
+    <t>546,900</t>
+  </si>
+  <si>
+    <t>646,900</t>
+  </si>
+  <si>
+    <t>mazda-cx30-camioneta-roja-flydown-perfil-v1</t>
+  </si>
+  <si>
+    <t>mazda-mexico-cx-5-flydown-perfil-v1</t>
+  </si>
+  <si>
+    <t>mazda-cx50-suv-verde-flydown-v1</t>
+  </si>
+  <si>
+    <t>mazda-cx70-flydown-perfil-v1</t>
+  </si>
+  <si>
+    <t>mazda-cx-90-flydown-rojo-artesano-inclinado-v1</t>
+  </si>
+  <si>
+    <t>mazda-mx-5-auto-rojo-deportivo-perfil-v1</t>
+  </si>
+  <si>
+    <t>auto-mazda-mx-5-rf-gris-titanio-perfil-v1</t>
+  </si>
+  <si>
+    <t>mazda-cx-3-flydown-perfil-v1</t>
+  </si>
+  <si>
+    <t>Carbon Edition MHEV</t>
+  </si>
+  <si>
     <t>Signature MHEV</t>
   </si>
   <si>
-    <t>340</t>
-  </si>
-  <si>
-    <t>369</t>
-  </si>
-  <si>
-    <t>3.3L</t>
-  </si>
-  <si>
-    <t>MAZDA CX-70</t>
-  </si>
-  <si>
-    <t>mazda3-hatchback-flydown-inclinado-v1</t>
-  </si>
-  <si>
-    <t>280</t>
-  </si>
-  <si>
-    <t>332</t>
-  </si>
-  <si>
-    <t>552,900</t>
-  </si>
-  <si>
-    <t>mazda-cx-30-flydown-perfil-v2</t>
-  </si>
-  <si>
-    <t>mazda-cx-50-flydown-v2</t>
-  </si>
-  <si>
-    <t>mazda-mazda2-sedan-rojo-perfil-v1</t>
-  </si>
-  <si>
-    <t>automovil-mazda2-hatchback-rojo-costado</t>
-  </si>
-  <si>
-    <t>mazda-mexico-cx-3-flydown-perfil-v1</t>
-  </si>
-  <si>
-    <t>mazda3-sedan-flydown-perfil-v2</t>
-  </si>
-  <si>
-    <t>mazda-cx-90-flydown-rojo-artesano-inclinado-v1.png</t>
-  </si>
-  <si>
-    <t>TRUE</t>
-  </si>
-  <si>
-    <t>1,061,000</t>
-  </si>
-  <si>
-    <t>330,900</t>
-  </si>
-  <si>
-    <t>370,900</t>
-  </si>
-  <si>
-    <t>398,900</t>
-  </si>
-  <si>
-    <t>403,900</t>
-  </si>
-  <si>
-    <t>442,900</t>
-  </si>
-  <si>
-    <t>482,900</t>
-  </si>
-  <si>
-    <t>458,900</t>
-  </si>
-  <si>
-    <t>498,900</t>
-  </si>
-  <si>
-    <t>568,900</t>
-  </si>
-  <si>
-    <t>391,900</t>
-  </si>
-  <si>
-    <t>421,900</t>
-  </si>
-  <si>
-    <t>441,900</t>
-  </si>
-  <si>
-    <t>471,900</t>
-  </si>
-  <si>
-    <t>517,900</t>
-  </si>
-  <si>
-    <t>557,900</t>
-  </si>
-  <si>
-    <t>551,900</t>
-  </si>
-  <si>
-    <t>611,900</t>
-  </si>
-  <si>
-    <t>681,900</t>
-  </si>
-  <si>
-    <t>818,900</t>
-  </si>
-  <si>
-    <t>961,000</t>
-  </si>
-  <si>
-    <t>529,900</t>
-  </si>
-  <si>
-    <t>629,900</t>
-  </si>
-  <si>
-    <t>mazda-cx-70-racks-flydown-inclinado-v1</t>
-  </si>
-  <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>PICKUPS</t>
-  </si>
-  <si>
-    <t>MAZDA BT-50</t>
-  </si>
-  <si>
-    <t>mazda-bt-50-roja-flydown-inclinado-v2</t>
-  </si>
-  <si>
-    <t>3.0L</t>
-  </si>
-  <si>
-    <t>300,900</t>
-  </si>
-  <si>
-    <t>799,900</t>
+    <t>Signature MHEV (Asientos Capitán)</t>
   </si>
 </sst>
 </file>
@@ -713,34 +722,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="2" max="2" width="47.1875" customWidth="1"/>
+    <col min="3" max="3" width="11.75" customWidth="1"/>
+    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.75" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.25" customWidth="1"/>
     <col min="8" max="8" width="9" style="1"/>
     <col min="9" max="9" width="4" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.77734375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.21875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.21875" customWidth="1"/>
+    <col min="10" max="10" width="8.75" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.25" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.25" customWidth="1"/>
     <col min="13" max="13" width="9" style="1"/>
-    <col min="14" max="15" width="8.77734375" style="1"/>
-    <col min="16" max="16" width="9.21875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.77734375" customWidth="1"/>
+    <col min="14" max="15" width="8.75" style="1"/>
+    <col min="16" max="16" width="9.25" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.75" customWidth="1"/>
     <col min="18" max="18" width="9" style="1"/>
-    <col min="19" max="21" width="8.77734375" style="1"/>
-    <col min="22" max="22" width="13.88671875" customWidth="1"/>
-    <col min="25" max="25" width="8.77734375" customWidth="1"/>
-    <col min="27" max="27" width="10.109375" customWidth="1"/>
-    <col min="32" max="32" width="13.88671875" customWidth="1"/>
+    <col min="19" max="21" width="8.75" style="1"/>
+    <col min="22" max="22" width="13.875" customWidth="1"/>
+    <col min="25" max="25" width="8.75" customWidth="1"/>
+    <col min="27" max="27" width="10.125" customWidth="1"/>
+    <col min="32" max="32" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -855,10 +864,10 @@
     </row>
     <row r="2" spans="1:36">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>64</v>
@@ -870,13 +879,13 @@
         <v>36</v>
       </c>
       <c r="F2">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="G2" t="s">
         <v>37</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>38</v>
@@ -891,7 +900,7 @@
         <v>41</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>38</v>
@@ -906,7 +915,7 @@
         <v>49</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>38</v>
@@ -921,13 +930,13 @@
         <v>50</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>48</v>
@@ -935,10 +944,10 @@
     </row>
     <row r="3" spans="1:36">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>64</v>
@@ -950,13 +959,13 @@
         <v>43</v>
       </c>
       <c r="F3">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="G3" t="s">
         <v>41</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>38</v>
@@ -971,7 +980,7 @@
         <v>49</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>38</v>
@@ -986,13 +995,13 @@
         <v>50</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="U3" s="3" t="s">
         <v>48</v>
@@ -1003,10 +1012,10 @@
     </row>
     <row r="4" spans="1:36">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>64</v>
@@ -1018,13 +1027,13 @@
         <v>36</v>
       </c>
       <c r="F4">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="G4" t="s">
         <v>37</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>45</v>
@@ -1039,7 +1048,7 @@
         <v>41</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>45</v>
@@ -1054,7 +1063,7 @@
         <v>49</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>45</v>
@@ -1066,33 +1075,45 @@
         <v>46</v>
       </c>
       <c r="V4" t="s">
+        <v>42</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA4" t="s">
         <v>50</v>
       </c>
-      <c r="W4" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="X4" s="1" t="s">
+      <c r="AB4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AE4" t="s">
         <v>46</v>
       </c>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
     </row>
     <row r="5" spans="1:36">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>64</v>
@@ -1104,13 +1125,13 @@
         <v>43</v>
       </c>
       <c r="F5">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="G5" t="s">
         <v>41</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>45</v>
@@ -1125,7 +1146,7 @@
         <v>49</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>45</v>
@@ -1140,7 +1161,7 @@
         <v>50</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>51</v>
@@ -1159,10 +1180,10 @@
     </row>
     <row r="6" spans="1:36">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>65</v>
@@ -1174,13 +1195,13 @@
         <v>54</v>
       </c>
       <c r="F6">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="G6" t="s">
         <v>37</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>47</v>
@@ -1195,7 +1216,7 @@
         <v>41</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>47</v>
@@ -1213,10 +1234,10 @@
     </row>
     <row r="7" spans="1:36">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>65</v>
@@ -1228,13 +1249,13 @@
         <v>54</v>
       </c>
       <c r="F7">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="G7" t="s">
         <v>37</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>45</v>
@@ -1249,7 +1270,7 @@
         <v>41</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>45</v>
@@ -1264,7 +1285,7 @@
         <v>49</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>45</v>
@@ -1279,7 +1300,7 @@
         <v>50</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="X7" s="1" t="s">
         <v>51</v>
@@ -1293,10 +1314,10 @@
     </row>
     <row r="8" spans="1:36">
       <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>65</v>
@@ -1314,7 +1335,7 @@
         <v>41</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>58</v>
@@ -1329,7 +1350,7 @@
         <v>49</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>58</v>
@@ -1344,7 +1365,7 @@
         <v>50</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>51</v>
@@ -1362,10 +1383,10 @@
     </row>
     <row r="9" spans="1:36">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>65</v>
@@ -1377,13 +1398,13 @@
         <v>54</v>
       </c>
       <c r="F9">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>50</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>59</v>
@@ -1397,45 +1418,45 @@
     </row>
     <row r="10" spans="1:36">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E10" t="s">
         <v>54</v>
       </c>
       <c r="F10">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>123</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:36">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>65</v>
@@ -1447,36 +1468,51 @@
         <v>54</v>
       </c>
       <c r="F11">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:36">
       <c r="A12" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="E12" t="s">
         <v>54</v>
@@ -1488,24 +1524,24 @@
         <v>50</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>58</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:36">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>66</v>
@@ -1517,7 +1553,7 @@
         <v>54</v>
       </c>
       <c r="F13">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="G13" t="s">
         <v>41</v>
@@ -1537,10 +1573,10 @@
     </row>
     <row r="14" spans="1:36">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>66</v>
@@ -1552,7 +1588,7 @@
         <v>54</v>
       </c>
       <c r="F14">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="G14" t="s">
         <v>49</v>

</xml_diff>